<commit_message>
up file excel intellji thymeleaf
</commit_message>
<xml_diff>
--- a/Báo cáo prj3_NguyenVanThinh_K23cnt1.xlsx
+++ b/Báo cáo prj3_NguyenVanThinh_K23cnt1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\2310900101_NguyenVanThinh\K23CNT1-PRJ3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7C4782-4762-4B8E-AAD4-ADB6F08837A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB8FEB2-4591-41A1-B4A9-22B07EBC628F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FFEB5152-AC08-4C0D-A2E4-E99156457D8E}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="14016" windowHeight="12336" activeTab="2" xr2:uid="{FFEB5152-AC08-4C0D-A2E4-E99156457D8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="420">
   <si>
     <t>1. Giới thiệu tổng quan bài toán</t>
   </si>
@@ -1318,12 +1318,37 @@
       <t xml:space="preserve"> giúp tự động hóa các công việc:</t>
     </r>
   </si>
+  <si>
+    <t>Tuần 2</t>
+  </si>
+  <si>
+    <r>
+      <t>Tạo cơ sở dữ liệu M</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ý"/>
+      </rPr>
+      <t>ySQL workbench</t>
+    </r>
+  </si>
+  <si>
+    <t>Hoàn thiện controller,repository,service</t>
+  </si>
+  <si>
+    <t>Hoàn thiện templates admin ,user</t>
+  </si>
+  <si>
+    <t>Chạy thử trang admin, user</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1384,6 +1409,11 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ý"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1405,7 +1435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1433,6 +1463,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
@@ -4963,7 +4999,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E188F29-A014-4C37-A5C2-B18E5EB077BB}">
   <dimension ref="A1:B77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -5454,7 +5490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{655930F6-1AC6-4E62-8848-368E129622F8}">
   <dimension ref="A1:I173"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="R41" sqref="R41"/>
     </sheetView>
   </sheetViews>
@@ -8238,14 +8274,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2B103DF-EE58-49FB-84A2-FCA7E71D479B}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
+    <col min="2" max="2" width="33.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.44140625" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
@@ -8325,11 +8361,48 @@
         <v>412</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
-      <c r="J7" s="12"/>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>415</v>
+      </c>
+      <c r="B6" t="s">
+        <v>416</v>
+      </c>
+      <c r="C6" t="s">
+        <v>413</v>
+      </c>
+      <c r="D6" t="s">
+        <v>413</v>
+      </c>
+      <c r="F6" s="14">
+        <v>0.99</v>
+      </c>
+      <c r="G6" s="15">
+        <v>45999</v>
+      </c>
+      <c r="H6" s="15">
+        <v>46005</v>
+      </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="16" customFormat="1" ht="17.399999999999999" customHeight="1">
+      <c r="B7" s="18" t="s">
+        <v>417</v>
+      </c>
+      <c r="J7" s="17"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="B8" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="12"/>
+      <c r="B9" t="s">
+        <v>419</v>
+      </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="12"/>
@@ -8339,8 +8412,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix loginadmin , userbill ,adminbill ,database MYSQL worbench
</commit_message>
<xml_diff>
--- a/Báo cáo prj3_NguyenVanThinh_K23cnt1.xlsx
+++ b/Báo cáo prj3_NguyenVanThinh_K23cnt1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\2310900101_NguyenVanThinh\K23CNT1-PRJ3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB8FEB2-4591-41A1-B4A9-22B07EBC628F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA1483D-6545-455C-9FD9-FD8B0C907F7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="14016" windowHeight="12336" activeTab="2" xr2:uid="{FFEB5152-AC08-4C0D-A2E4-E99156457D8E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{FFEB5152-AC08-4C0D-A2E4-E99156457D8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="426">
   <si>
     <t>1. Giới thiệu tổng quan bài toán</t>
   </si>
@@ -1342,6 +1342,24 @@
   </si>
   <si>
     <t>Chạy thử trang admin, user</t>
+  </si>
+  <si>
+    <t>Tuần 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fix cở sở dữ liệu </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hoàn thiện các trang admin ,user,login admin </t>
+  </si>
+  <si>
+    <t>Thêm phần thanh toán online</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thông báo gửi về mail </t>
+  </si>
+  <si>
+    <t>Hoàn thiện báo cáo word</t>
   </si>
 </sst>
 </file>
@@ -1435,7 +1453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1464,8 +1482,6 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -4999,7 +5015,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E188F29-A014-4C37-A5C2-B18E5EB077BB}">
   <dimension ref="A1:B77"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -8275,7 +8291,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8362,7 +8378,7 @@
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" t="s">
+      <c r="A6" s="12" t="s">
         <v>415</v>
       </c>
       <c r="B6" t="s">
@@ -8387,11 +8403,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="16" customFormat="1" ht="17.399999999999999" customHeight="1">
-      <c r="B7" s="18" t="s">
+    <row r="7" spans="1:10" ht="17.399999999999999" customHeight="1">
+      <c r="B7" s="16" t="s">
         <v>417</v>
       </c>
-      <c r="J7" s="17"/>
+      <c r="J7" s="12"/>
     </row>
     <row r="8" spans="1:10">
       <c r="B8" t="s">
@@ -8402,6 +8418,50 @@
       <c r="A9" s="12"/>
       <c r="B9" t="s">
         <v>419</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="12" t="s">
+        <v>420</v>
+      </c>
+      <c r="B10" t="s">
+        <v>421</v>
+      </c>
+      <c r="C10" t="s">
+        <v>413</v>
+      </c>
+      <c r="D10" t="s">
+        <v>413</v>
+      </c>
+      <c r="F10" s="14"/>
+      <c r="G10" s="15">
+        <v>46006</v>
+      </c>
+      <c r="H10" s="15">
+        <v>46011</v>
+      </c>
+      <c r="I10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="B11" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="B12" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="B13" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="B14" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="16" spans="1:10">

</xml_diff>